<commit_message>
Wrote healthy life expectancy code
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Support Work/Healthy Life Expectancy/life-expectancy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E22F27B1-DB3B-4882-8C07-55DF60A610D2}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="11_F25DC773A252ABDACC1048C4315C7F365BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A2CA217-2669-4920-9DD2-564B5C7688E5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
-    <sheet name="data" sheetId="1" r:id="rId2"/>
+    <sheet name="pop_and_deaths" sheetId="1" r:id="rId2"/>
+    <sheet name="good_health" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="intNumber_of_DataRows">[1]Data!$O$1</definedName>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Age at Start of Interval</t>
   </si>
@@ -193,25 +194,47 @@
   <si>
     <t>Based on life expectancy template available here:</t>
   </si>
+  <si>
+    <t>Survey population (n_weighted base)</t>
+  </si>
+  <si>
+    <t>Survey population in good general health (n_weighted)</t>
+  </si>
+  <si>
+    <t>Unweighted base: Survey Population</t>
+  </si>
+  <si>
+    <t>Survey population in good health (n_unweighted)</t>
+  </si>
+  <si>
+    <t>Adjustment Factors (age-bands &lt;1 to 10-14, 85-89 to 90+)</t>
+  </si>
+  <si>
+    <t>Spop_w</t>
+  </si>
+  <si>
+    <t>Spop_gh_w</t>
+  </si>
+  <si>
+    <t>Spop</t>
+  </si>
+  <si>
+    <t>Spop_gh</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="?0"/>
-    <numFmt numFmtId="166" formatCode="???,??0"/>
-    <numFmt numFmtId="167" formatCode="??,??0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +291,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -289,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -413,90 +466,199 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -815,40 +977,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B669E7-5E5B-48F3-9C12-776251D77E09}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="5.7265625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="10"/>
+      <c r="A2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2"/>
@@ -856,54 +1018,95 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="18"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="18"/>
+      <c r="B8" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -911,245 +1114,942 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" activeCellId="1" sqref="B2:C21 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>0</v>
       </c>
-      <c r="B2" s="12">
-        <v>46886</v>
-      </c>
-      <c r="C2" s="14">
-        <v>307</v>
+      <c r="B2" s="50">
+        <v>1204096</v>
+      </c>
+      <c r="C2" s="50">
+        <v>5097</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="12">
-        <v>197911</v>
-      </c>
-      <c r="C3" s="14">
-        <v>39</v>
+      <c r="B3" s="50">
+        <v>4977412</v>
+      </c>
+      <c r="C3" s="50">
+        <v>870</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>5</v>
       </c>
-      <c r="B4" s="12">
-        <v>249134</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="50">
+        <v>5924907</v>
+      </c>
+      <c r="C4" s="50">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>10</v>
+      </c>
+      <c r="B5" s="50">
+        <v>5428148</v>
+      </c>
+      <c r="C5" s="50">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>15</v>
+      </c>
+      <c r="B6" s="50">
+        <v>5934244</v>
+      </c>
+      <c r="C6" s="50">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>20</v>
+      </c>
+      <c r="B7" s="50">
+        <v>6569549</v>
+      </c>
+      <c r="C7" s="50">
+        <v>3256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
-        <v>10</v>
-      </c>
-      <c r="B5" s="12">
-        <v>237067</v>
-      </c>
-      <c r="C5" s="14">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="13">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12">
-        <v>238610</v>
-      </c>
-      <c r="C6" s="14">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="13">
-        <v>20</v>
-      </c>
-      <c r="B7" s="12">
-        <v>314963</v>
-      </c>
-      <c r="C7" s="14">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="13">
-        <v>25</v>
-      </c>
-      <c r="B8" s="12">
-        <v>292358</v>
-      </c>
-      <c r="C8" s="14">
-        <v>128</v>
+      <c r="B8" s="50">
+        <v>6598118</v>
+      </c>
+      <c r="C8" s="50">
+        <v>4101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <v>30</v>
       </c>
-      <c r="B9" s="12">
-        <v>249313</v>
-      </c>
-      <c r="C9" s="14">
-        <v>176</v>
+      <c r="B9" s="50">
+        <v>6491309</v>
+      </c>
+      <c r="C9" s="50">
+        <v>5375</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="13">
+      <c r="A10" s="11">
         <v>35</v>
       </c>
-      <c r="B10" s="12">
-        <v>228239</v>
-      </c>
-      <c r="C10" s="14">
-        <v>262</v>
+      <c r="B10" s="50">
+        <v>5993478</v>
+      </c>
+      <c r="C10" s="50">
+        <v>7207</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="13">
+      <c r="A11" s="11">
         <v>40</v>
       </c>
-      <c r="B11" s="12">
-        <v>201799</v>
-      </c>
-      <c r="C11" s="14">
-        <v>389</v>
+      <c r="B11" s="50">
+        <v>6521186</v>
+      </c>
+      <c r="C11" s="50">
+        <v>11604</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="13">
+      <c r="A12" s="11">
         <v>45</v>
       </c>
-      <c r="B12" s="12">
-        <v>200207</v>
-      </c>
-      <c r="C12" s="14">
-        <v>543</v>
+      <c r="B12" s="50">
+        <v>6895826</v>
+      </c>
+      <c r="C12" s="50">
+        <v>17689</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>50</v>
       </c>
-      <c r="B13" s="12">
-        <v>196723</v>
-      </c>
-      <c r="C13" s="14">
-        <v>837</v>
+      <c r="B13" s="50">
+        <v>6603740</v>
+      </c>
+      <c r="C13" s="50">
+        <v>24782</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>55</v>
       </c>
-      <c r="B14" s="12">
-        <v>178068</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1095</v>
+      <c r="B14" s="50">
+        <v>5703149</v>
+      </c>
+      <c r="C14" s="50">
+        <v>33998</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>60</v>
       </c>
-      <c r="B15" s="12">
-        <v>145663</v>
-      </c>
-      <c r="C15" s="14">
-        <v>1534</v>
+      <c r="B15" s="50">
+        <v>5167986</v>
+      </c>
+      <c r="C15" s="50">
+        <v>49954</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>65</v>
       </c>
-      <c r="B16" s="12">
-        <v>124071</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1856</v>
+      <c r="B16" s="50">
+        <v>5183699</v>
+      </c>
+      <c r="C16" s="50">
+        <v>75707</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>70</v>
       </c>
-      <c r="B17" s="12">
-        <v>108735</v>
-      </c>
-      <c r="C17" s="14">
-        <v>2577</v>
+      <c r="B17" s="50">
+        <v>3748158</v>
+      </c>
+      <c r="C17" s="50">
+        <v>91712</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>75</v>
       </c>
-      <c r="B18" s="12">
-        <v>82744</v>
-      </c>
-      <c r="C18" s="14">
-        <v>3188</v>
+      <c r="B18" s="50">
+        <v>2925977</v>
+      </c>
+      <c r="C18" s="50">
+        <v>120003</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>80</v>
       </c>
-      <c r="B19" s="12">
-        <v>65470</v>
-      </c>
-      <c r="C19" s="14">
-        <v>4276</v>
+      <c r="B19" s="50">
+        <v>1994844</v>
+      </c>
+      <c r="C19" s="50">
+        <v>145110</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>85</v>
       </c>
-      <c r="B20" s="12">
-        <v>41606</v>
-      </c>
-      <c r="C20" s="14">
-        <v>4613</v>
+      <c r="B20" s="50">
+        <v>1065940</v>
+      </c>
+      <c r="C20" s="50">
+        <v>137456</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="15">
+      <c r="A21" s="12">
         <v>90</v>
       </c>
-      <c r="B21" s="16">
-        <v>24148</v>
-      </c>
-      <c r="C21" s="17">
-        <v>5157</v>
+      <c r="B21" s="50">
+        <v>469452</v>
+      </c>
+      <c r="C21" s="50">
+        <v>111465</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5FEACF-F953-41AC-ADBF-803550F15172}">
+  <dimension ref="A1:I64"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.08984375" style="29" customWidth="1"/>
+    <col min="3" max="5" width="22.36328125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="20" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="10">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31">
+        <f>$Y$6</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="18">
+        <v>11563</v>
+      </c>
+      <c r="F2" s="32">
+        <v>1.0040010443169987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31">
+        <f>$Y$6</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="18">
+        <v>11563</v>
+      </c>
+      <c r="F3" s="33">
+        <v>1.0024781127170845</v>
+      </c>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>5</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31">
+        <f>$Y$6</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="18">
+        <v>11563</v>
+      </c>
+      <c r="F4" s="33">
+        <v>1.0019823731012256</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>10</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31">
+        <f>$Y$6</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="18">
+        <v>11563</v>
+      </c>
+      <c r="F5" s="33">
+        <v>1.0056388585125775</v>
+      </c>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>15</v>
+      </c>
+      <c r="B6" s="34">
+        <v>1493072</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1401638</v>
+      </c>
+      <c r="D6" s="18">
+        <v>12311</v>
+      </c>
+      <c r="E6" s="18">
+        <v>11563</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>20</v>
+      </c>
+      <c r="B7" s="34">
+        <v>2063660</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1885088</v>
+      </c>
+      <c r="D7" s="18">
+        <v>12768</v>
+      </c>
+      <c r="E7" s="18">
+        <v>11638</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>25</v>
+      </c>
+      <c r="B8" s="34">
+        <v>2088111</v>
+      </c>
+      <c r="C8" s="18">
+        <v>1874814</v>
+      </c>
+      <c r="D8" s="18">
+        <v>12944</v>
+      </c>
+      <c r="E8" s="18">
+        <v>11543</v>
+      </c>
+      <c r="F8" s="35"/>
+    </row>
+    <row r="9" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>30</v>
+      </c>
+      <c r="B9" s="34">
+        <v>2055699</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1824483</v>
+      </c>
+      <c r="D9" s="18">
+        <v>14882</v>
+      </c>
+      <c r="E9" s="18">
+        <v>13151</v>
+      </c>
+      <c r="F9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>35</v>
+      </c>
+      <c r="B10" s="34">
+        <v>1914037</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1656748</v>
+      </c>
+      <c r="D10" s="18">
+        <v>15212</v>
+      </c>
+      <c r="E10" s="18">
+        <v>13095</v>
+      </c>
+      <c r="F10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>40</v>
+      </c>
+      <c r="B11" s="34">
+        <v>2083071</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1735853</v>
+      </c>
+      <c r="D11" s="18">
+        <v>17372</v>
+      </c>
+      <c r="E11" s="18">
+        <v>14394</v>
+      </c>
+      <c r="F11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>45</v>
+      </c>
+      <c r="B12" s="34">
+        <v>2219522</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1776239</v>
+      </c>
+      <c r="D12" s="18">
+        <v>18637</v>
+      </c>
+      <c r="E12" s="18">
+        <v>14846</v>
+      </c>
+      <c r="F12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>50</v>
+      </c>
+      <c r="B13" s="34">
+        <v>2135486</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1630347</v>
+      </c>
+      <c r="D13" s="18">
+        <v>18426</v>
+      </c>
+      <c r="E13" s="18">
+        <v>13952</v>
+      </c>
+      <c r="F13" s="35"/>
+    </row>
+    <row r="14" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <v>55</v>
+      </c>
+      <c r="B14" s="34">
+        <v>1849288</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1313112</v>
+      </c>
+      <c r="D14" s="18">
+        <v>17158</v>
+      </c>
+      <c r="E14" s="18">
+        <v>12070</v>
+      </c>
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="10">
+        <v>60</v>
+      </c>
+      <c r="B15" s="34">
+        <v>1684861</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1120845</v>
+      </c>
+      <c r="D15" s="18">
+        <v>17249</v>
+      </c>
+      <c r="E15" s="18">
+        <v>11350</v>
+      </c>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="10">
+        <v>65</v>
+      </c>
+      <c r="B16" s="34">
+        <v>1691020</v>
+      </c>
+      <c r="C16" s="18">
+        <v>1093830</v>
+      </c>
+      <c r="D16" s="18">
+        <v>18096</v>
+      </c>
+      <c r="E16" s="18">
+        <v>11641</v>
+      </c>
+      <c r="F16" s="35"/>
+    </row>
+    <row r="17" spans="1:6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="10">
+        <v>70</v>
+      </c>
+      <c r="B17" s="34">
+        <v>1209519</v>
+      </c>
+      <c r="C17" s="18">
+        <v>737160</v>
+      </c>
+      <c r="D17" s="18">
+        <v>13519</v>
+      </c>
+      <c r="E17" s="18">
+        <v>8229</v>
+      </c>
+      <c r="F17" s="35"/>
+    </row>
+    <row r="18" spans="1:6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="10">
+        <v>75</v>
+      </c>
+      <c r="B18" s="34">
+        <v>841721</v>
+      </c>
+      <c r="C18" s="18">
+        <v>465478</v>
+      </c>
+      <c r="D18" s="18">
+        <v>6602</v>
+      </c>
+      <c r="E18" s="18">
+        <v>3617</v>
+      </c>
+      <c r="F18" s="35"/>
+    </row>
+    <row r="19" spans="1:6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="10">
+        <v>80</v>
+      </c>
+      <c r="B19" s="34">
+        <v>480775</v>
+      </c>
+      <c r="C19" s="18">
+        <v>241233</v>
+      </c>
+      <c r="D19" s="18">
+        <v>3810</v>
+      </c>
+      <c r="E19" s="18">
+        <v>1899</v>
+      </c>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="20" spans="1:6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="10">
+        <v>85</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18">
+        <f>$Y$19</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="18">
+        <v>1899</v>
+      </c>
+      <c r="F20" s="36">
+        <v>0.81743857566979328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="12">
+        <v>90</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38">
+        <f>$Y$19</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="38">
+        <v>1899</v>
+      </c>
+      <c r="F21" s="39">
+        <v>0.86951010549961627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+    </row>
+    <row r="44" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+    </row>
+    <row r="59" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+    </row>
+    <row r="61" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+    </row>
+    <row r="63" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27:F27" r:id="rId1" display="ONS Interim Life Tables - calculated over three years, available from the Office for National Statistics website." xr:uid="{ED1C1A1D-30E2-4F56-9C63-9C2615578EED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>